<commit_message>
Addition of a standard tire model for Hoosier R20 16x7.5 tires, with this model included in the standard Excel car model template.
</commit_message>
<xml_diff>
--- a/LapsimAndYMD/Templates/FSAE_QueensRacingVEHICLE_Template.xlsx
+++ b/LapsimAndYMD/Templates/FSAE_QueensRacingVEHICLE_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7675256453cb331e/Documents/Queens/Formula SAE/QueensRacing_Modelling/VD/LapsimAndYMD/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7675256453cb331e/Documents/Queens/Formula SAE/VehicleDynamics_Modelling/LapsimAndYMD/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2812" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A7E65B-A22B-49CE-BE40-18F4BE1314CC}"/>
+  <xr:revisionPtr revIDLastSave="2813" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0A13224-38DB-4ECB-A51D-EBF6B6EEF781}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -307,9 +307,6 @@
     <t>Should be positive</t>
   </si>
   <si>
-    <t>big_tire</t>
-  </si>
-  <si>
     <t>Should be a string of the .mat file with processed tire data, without the .mat file extension</t>
   </si>
   <si>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>QueensRacingXX</t>
+  </si>
+  <si>
+    <t>Hoosier16x7p5</t>
   </si>
 </sst>
 </file>
@@ -1074,19 +1074,19 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="123.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="123.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
@@ -1111,27 +1111,27 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>7</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
       <c r="B5" s="18" t="s">
         <v>31</v>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="41"/>
       <c r="B6" s="22" t="s">
         <v>32</v>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="E6" s="25"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>6</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="2" t="s">
         <v>33</v>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="46"/>
       <c r="B9" s="9" t="s">
         <v>34</v>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>73</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
         <v>8</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -1262,7 +1262,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="2" t="s">
         <v>24</v>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="2" t="s">
         <v>11</v>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="E14" s="13"/>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="42"/>
       <c r="B15" s="9" t="s">
         <v>14</v>
@@ -1303,7 +1303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>35</v>
       </c>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="2" t="s">
         <v>37</v>
@@ -1333,7 +1333,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="2" t="s">
         <v>16</v>
@@ -1348,7 +1348,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="45"/>
       <c r="B19" s="22" t="s">
         <v>17</v>
@@ -1363,7 +1363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="39" t="s">
         <v>40</v>
       </c>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="2" t="s">
         <v>41</v>
@@ -1393,7 +1393,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="2" t="s">
         <v>42</v>
@@ -1408,7 +1408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="2" t="s">
         <v>43</v>
@@ -1423,7 +1423,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="2" t="s">
         <v>44</v>
@@ -1438,7 +1438,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="41"/>
       <c r="B25" s="22" t="s">
         <v>76</v>
@@ -1454,7 +1454,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="22" t="s">
         <v>77</v>
@@ -1469,7 +1469,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="41"/>
       <c r="B27" s="22" t="s">
         <v>82</v>
@@ -1484,22 +1484,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="42"/>
       <c r="B28" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
         <v>48</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="38"/>
       <c r="B30" s="2" t="s">
         <v>49</v>
@@ -1531,7 +1531,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="46"/>
       <c r="B31" s="9" t="s">
         <v>51</v>
@@ -1546,7 +1546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>54</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="38"/>
       <c r="B33" s="27" t="s">
         <v>57</v>
@@ -1576,7 +1576,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="38"/>
       <c r="B34" s="27" t="s">
         <v>60</v>
@@ -1591,7 +1591,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="38"/>
       <c r="B35" s="27" t="s">
         <v>62</v>
@@ -1606,7 +1606,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="38"/>
       <c r="B36" s="27" t="s">
         <v>64</v>
@@ -1621,7 +1621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="38"/>
       <c r="B37" s="2" t="s">
         <v>65</v>
@@ -1636,7 +1636,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="38"/>
       <c r="B38" s="2" t="s">
         <v>66</v>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="E38" s="13"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="38"/>
       <c r="B39" s="31" t="s">
         <v>67</v>
@@ -1662,7 +1662,7 @@
       </c>
       <c r="E39" s="13"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="38"/>
       <c r="B40" s="31" t="s">
         <v>68</v>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="E40" s="13"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="38"/>
       <c r="B41" s="31" t="s">
         <v>69</v>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="E41" s="13"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="38"/>
       <c r="B42" s="31" t="s">
         <v>70</v>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="38"/>
       <c r="B43" s="31" t="s">
         <v>71</v>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="E43" s="13"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="38"/>
       <c r="B44" s="31" t="s">
         <v>72</v>
@@ -1749,13 +1749,13 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1500</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2500</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3000</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3500</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4000</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4500</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5000</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5500</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6000</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6500</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7000</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7500</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8000</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8500</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9000</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>9500</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10000</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10500</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11000</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11500</v>
       </c>

</xml_diff>

<commit_message>
Updated all scripts to no longer make use of global variables for vehicle modelling, but instead reference a vehicle structure. This will improve the code usability when performing sensitivity analyses using yaw moment diagrams, and allow users to make better use of the parfor command, by not using the xlswrite command. Lapsim documentation has also been updated to reflect these changes to the global variable modification, as well as the revised yaw moment diagram method. Additionally, QueensRacingYMD has been removed, as it has become obsolete with these changes. Now to run a YMD, the user should generate a vehicle model using readCarFromExcel, then run a YMD using extractYMD and its function inputs. This should reduce superfluous code.
</commit_message>
<xml_diff>
--- a/LapsimAndYMD/Templates/FSAE_QueensRacingVEHICLE_Template.xlsx
+++ b/LapsimAndYMD/Templates/FSAE_QueensRacingVEHICLE_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7675256453cb331e/Documents/Queens/Formula SAE/VehicleDynamics_Modelling/LapsimAndYMD/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2813" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0A13224-38DB-4ECB-A51D-EBF6B6EEF781}"/>
+  <xr:revisionPtr revIDLastSave="2816" documentId="11_88FF5E97F77A6102EC0E57248F669B8764C9C532" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C46C581-0D04-43FD-8CFF-E1DF266CDEED}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,8 +1444,8 @@
         <v>76</v>
       </c>
       <c r="C25" s="23">
-        <f>18.3/2*25.4</f>
-        <v>232.41</v>
+        <f>16.2/2*25.4</f>
+        <v>205.73999999999998</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>39</v>

</xml_diff>